<commit_message>
adiciona documentação e melhorias nas funções de manipulação de JSON e XLSX
</commit_message>
<xml_diff>
--- a/data/input_model.xlsx
+++ b/data/input_model.xlsx
@@ -7,12 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="employees" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="company" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Chaves Principais" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="employees" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="company" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'employees'!$A$1:$I$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'company'!$A$1:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Chaves Principais'!$A$1:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'employees'!$A$1:$I$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'company'!$A$1:$K$13</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -33,12 +35,24 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -98,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -112,10 +126,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -485,6 +505,98 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Chave primária</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Significado</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Observações</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>company</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>dict</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>employees</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>list</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -560,7 +672,7 @@
       <c r="B2" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>int</t>
         </is>
@@ -575,7 +687,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -607,7 +719,7 @@
           <t>Sales</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
+      <c r="C3" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -622,7 +734,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -654,7 +766,7 @@
           <t>john.doe@example.com</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -669,7 +781,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F4" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -701,7 +813,7 @@
           <t>John Doe</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -716,7 +828,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -743,7 +855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -846,7 +958,7 @@
       <c r="D2" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>int</t>
         </is>
@@ -861,7 +973,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -883,8 +995,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="n"/>
-      <c r="B3" s="7" t="n"/>
+      <c r="A3" s="9" t="n"/>
+      <c r="B3" s="9" t="n"/>
       <c r="C3" s="3" t="inlineStr">
         <is>
           <t>manager</t>
@@ -895,7 +1007,7 @@
           <t>Charlie Black</t>
         </is>
       </c>
-      <c r="E3" s="6" t="inlineStr">
+      <c r="E3" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -910,7 +1022,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H3" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -932,8 +1044,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="n"/>
-      <c r="B4" s="8" t="n"/>
+      <c r="A4" s="9" t="n"/>
+      <c r="B4" s="10" t="n"/>
       <c r="C4" s="3" t="inlineStr">
         <is>
           <t>projects</t>
@@ -944,7 +1056,7 @@
           <t>2023-12-31</t>
         </is>
       </c>
-      <c r="E4" s="6" t="inlineStr">
+      <c r="E4" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -959,7 +1071,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="H4" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -981,7 +1093,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="n"/>
+      <c r="A5" s="9" t="n"/>
       <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Marketing</t>
@@ -995,7 +1107,7 @@
       <c r="D5" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>int</t>
         </is>
@@ -1010,7 +1122,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="H5" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1032,8 +1144,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="n"/>
-      <c r="B6" s="8" t="n"/>
+      <c r="A6" s="9" t="n"/>
+      <c r="B6" s="10" t="n"/>
       <c r="C6" s="3" t="inlineStr">
         <is>
           <t>manager</t>
@@ -1044,7 +1156,7 @@
           <t>Bob White</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -1059,7 +1171,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H6" s="5" t="inlineStr">
+      <c r="H6" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1081,7 +1193,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="n"/>
+      <c r="A7" s="9" t="n"/>
       <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Sales</t>
@@ -1095,7 +1207,7 @@
       <c r="D7" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>int</t>
         </is>
@@ -1110,7 +1222,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H7" s="5" t="inlineStr">
+      <c r="H7" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1132,8 +1244,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="n"/>
-      <c r="B8" s="8" t="n"/>
+      <c r="A8" s="10" t="n"/>
+      <c r="B8" s="10" t="n"/>
       <c r="C8" s="3" t="inlineStr">
         <is>
           <t>manager</t>
@@ -1144,7 +1256,7 @@
           <t>Alice Brown</t>
         </is>
       </c>
-      <c r="E8" s="6" t="inlineStr">
+      <c r="E8" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -1159,7 +1271,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H8" s="5" t="inlineStr">
+      <c r="H8" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1201,7 +1313,7 @@
           <t>123 Tech Street</t>
         </is>
       </c>
-      <c r="E9" s="6" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -1216,7 +1328,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H9" s="5" t="inlineStr">
+      <c r="H9" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1238,19 +1350,19 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
           <t>city</t>
         </is>
       </c>
-      <c r="C10" s="7" t="n"/>
+      <c r="C10" s="9" t="n"/>
       <c r="D10" s="3" t="inlineStr">
         <is>
           <t>Tech City</t>
         </is>
       </c>
-      <c r="E10" s="6" t="inlineStr">
+      <c r="E10" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -1265,7 +1377,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H10" s="5" t="inlineStr">
+      <c r="H10" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1287,19 +1399,19 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="n"/>
+      <c r="A11" s="9" t="n"/>
       <c r="B11" s="3" t="inlineStr">
         <is>
           <t>country</t>
         </is>
       </c>
-      <c r="C11" s="7" t="n"/>
+      <c r="C11" s="9" t="n"/>
       <c r="D11" s="3" t="inlineStr">
         <is>
           <t>Techland</t>
         </is>
       </c>
-      <c r="E11" s="6" t="inlineStr">
+      <c r="E11" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -1314,7 +1426,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H11" s="5" t="inlineStr">
+      <c r="H11" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1336,19 +1448,19 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="n"/>
+      <c r="A12" s="10" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
           <t>postal_code</t>
         </is>
       </c>
-      <c r="C12" s="7" t="n"/>
+      <c r="C12" s="9" t="n"/>
       <c r="D12" s="3" t="inlineStr">
         <is>
           <t>12345</t>
         </is>
       </c>
-      <c r="E12" s="6" t="inlineStr">
+      <c r="E12" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -1363,7 +1475,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H12" s="5" t="inlineStr">
+      <c r="H12" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>
@@ -1395,13 +1507,13 @@
           <t>---</t>
         </is>
       </c>
-      <c r="C13" s="8" t="n"/>
+      <c r="C13" s="10" t="n"/>
       <c r="D13" s="3" t="inlineStr">
         <is>
           <t>Tech Solutions</t>
         </is>
       </c>
-      <c r="E13" s="6" t="inlineStr">
+      <c r="E13" s="8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
@@ -1416,7 +1528,7 @@
           <t>---</t>
         </is>
       </c>
-      <c r="H13" s="5" t="inlineStr">
+      <c r="H13" s="7" t="inlineStr">
         <is>
           <t>SIM</t>
         </is>

</xml_diff>